<commit_message>
random repo update to sync work between devices
</commit_message>
<xml_diff>
--- a/sem6/krypto/236382_lab1.xlsx
+++ b/sem6/krypto/236382_lab1.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blasz\OneDrive - Politechnika Łódzka\sem6_\krypto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blasz\work\studia\sem6\krypto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{C122FDCE-F744-404A-A4F2-C3CD61707499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A9B4A9-0759-48A5-83E6-4E5B74175F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>problem plecakowy</t>
   </si>
@@ -181,12 +182,51 @@
   </si>
   <si>
     <t>KP</t>
+  </si>
+  <si>
+    <t>p,q</t>
+  </si>
+  <si>
+    <t>pierwsze</t>
+  </si>
+  <si>
+    <t>256&lt;=</t>
+  </si>
+  <si>
+    <t>&lt;=512</t>
+  </si>
+  <si>
+    <t>n=</t>
+  </si>
+  <si>
+    <t>p*q</t>
+  </si>
+  <si>
+    <t>Fi</t>
+  </si>
+  <si>
+    <t>(p-1)(q-1)</t>
+  </si>
+  <si>
+    <t>e=</t>
+  </si>
+  <si>
+    <t>NWD(e, Fi)=1 ???</t>
+  </si>
+  <si>
+    <t>e*d mod Fi=1</t>
+  </si>
+  <si>
+    <t>d taka że</t>
+  </si>
+  <si>
+    <t>to szukamy d:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -238,9 +278,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -278,7 +318,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -384,7 +424,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -526,18 +566,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,7 +627,7 @@
         <v>2</v>
       </c>
       <c r="K3" s="1">
-        <f>MID($R$2,$I3,1)*1</f>
+        <f t="shared" ref="K3:K10" si="0">MID($R$2,$I3,1)*1</f>
         <v>1</v>
       </c>
       <c r="L3">
@@ -629,15 +669,15 @@
         <v>5</v>
       </c>
       <c r="K4" s="1">
-        <f>MID($R$2,$I4,1)*1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L10" si="0">K4*J4</f>
+        <f t="shared" ref="L4:L10" si="1">K4*J4</f>
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M10" si="1">MOD($H$21*I4,$H$20)</f>
+        <f t="shared" ref="M4:M10" si="2">MOD($H$21*I4,$H$20)</f>
         <v>354</v>
       </c>
       <c r="O4">
@@ -659,15 +699,15 @@
         <v>11</v>
       </c>
       <c r="K5" s="1">
-        <f>MID($R$2,$I5,1)*1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="M5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>531</v>
       </c>
       <c r="O5">
@@ -686,15 +726,15 @@
         <v>23</v>
       </c>
       <c r="K6" s="1">
-        <f>MID($R$2,$I6,1)*1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="M6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>708</v>
       </c>
       <c r="O6">
@@ -716,15 +756,15 @@
         <v>50</v>
       </c>
       <c r="K7" s="1">
-        <f>MID($R$2,$I7,1)*1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>885</v>
       </c>
       <c r="O7">
@@ -743,15 +783,15 @@
         <v>105</v>
       </c>
       <c r="K8" s="1">
-        <f>MID($R$2,$I8,1)*1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>105</v>
       </c>
       <c r="M8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="O8">
@@ -770,15 +810,15 @@
         <v>230</v>
       </c>
       <c r="K9" s="1">
-        <f>MID($R$2,$I9,1)*1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>230</v>
       </c>
       <c r="M9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>226</v>
       </c>
       <c r="O9">
@@ -797,15 +837,15 @@
         <v>477</v>
       </c>
       <c r="K10" s="1">
-        <f>MID($R$2,$I10,1)*1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>477</v>
       </c>
       <c r="M10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>403</v>
       </c>
       <c r="O10">
@@ -924,7 +964,7 @@
         <v>230</v>
       </c>
       <c r="M17" s="1">
-        <f t="shared" ref="M17:M23" si="2">MOD($H$21*L17,$H$20)</f>
+        <f t="shared" ref="M17:M23" si="3">MOD($H$21*L17,$H$20)</f>
         <v>190</v>
       </c>
       <c r="N17">
@@ -936,7 +976,7 @@
         <v>133</v>
       </c>
       <c r="P17">
-        <f t="shared" ref="P17:P23" si="3">IF(O17&gt;=L17,1,0)</f>
+        <f t="shared" ref="P17:P23" si="4">IF(O17&gt;=L17,1,0)</f>
         <v>0</v>
       </c>
       <c r="S17" t="s">
@@ -958,7 +998,7 @@
         <v>105</v>
       </c>
       <c r="M18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>351</v>
       </c>
       <c r="N18">
@@ -966,11 +1006,11 @@
         <v>1</v>
       </c>
       <c r="O18">
-        <f t="shared" ref="O18:O23" si="4">O17-P17*L17</f>
+        <f t="shared" ref="O18:O23" si="5">O17-P17*L17</f>
         <v>133</v>
       </c>
       <c r="P18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -982,7 +1022,7 @@
         <v>50</v>
       </c>
       <c r="M19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>746</v>
       </c>
       <c r="N19">
@@ -990,11 +1030,11 @@
         <v>0</v>
       </c>
       <c r="O19">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="P19">
         <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="P19">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1015,7 +1055,7 @@
         <v>23</v>
       </c>
       <c r="M20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="N20">
@@ -1023,11 +1063,11 @@
         <v>1</v>
       </c>
       <c r="O20">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="P20">
         <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="P20">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -1048,7 +1088,7 @@
         <v>11</v>
       </c>
       <c r="M21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>934</v>
       </c>
       <c r="N21">
@@ -1056,11 +1096,11 @@
         <v>0</v>
       </c>
       <c r="O21">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="P21">
         <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="P21">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1076,7 +1116,7 @@
         <v>5</v>
       </c>
       <c r="M22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>885</v>
       </c>
       <c r="N22">
@@ -1084,11 +1124,11 @@
         <v>1</v>
       </c>
       <c r="O22">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="P22">
         <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="P22">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -1109,7 +1149,7 @@
         <v>2</v>
       </c>
       <c r="M23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>354</v>
       </c>
       <c r="N23">
@@ -1117,11 +1157,11 @@
         <v>0</v>
       </c>
       <c r="O23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P23">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P23">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1152,4 +1192,78 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{778629B3-261E-42FE-8CDB-072C021EC8EF}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5">
+        <v>65537</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>